<commit_message>
updated invoice data Wed Dec 16 13:21:07 PST 2015
</commit_message>
<xml_diff>
--- a/Rooms&Services.xlsx
+++ b/Rooms&Services.xlsx
@@ -16847,7 +16847,7 @@
         <v>834</v>
       </c>
       <c r="M320" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="N320">
         <v>110</v>
@@ -20773,7 +20773,7 @@
         <v>823</v>
       </c>
       <c r="K411" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="L411" t="s">
         <v>834</v>
@@ -22739,7 +22739,7 @@
         <v>835</v>
       </c>
       <c r="M456" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="N456">
         <v>225</v>
@@ -27750,7 +27750,7 @@
         <v>823</v>
       </c>
       <c r="K572" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="L572" t="s">
         <v>834</v>
@@ -31255,7 +31255,7 @@
         <v>688</v>
       </c>
       <c r="D69" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="E69">
         <v>40</v>
@@ -40863,7 +40863,7 @@
         <v>709</v>
       </c>
       <c r="D297" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="E297">
         <v>30</v>
@@ -54200,7 +54200,7 @@
         <v>834</v>
       </c>
       <c r="M613" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="N613">
         <v>50</v>
@@ -54242,7 +54242,7 @@
         <v>834</v>
       </c>
       <c r="M614" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="N614">
         <v>250</v>
@@ -54257,7 +54257,7 @@
         <v>546</v>
       </c>
       <c r="D615" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="E615">
         <v>40</v>
@@ -54284,7 +54284,7 @@
         <v>834</v>
       </c>
       <c r="M615" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="N615">
         <v>40</v>
@@ -60745,7 +60745,7 @@
         <v>823</v>
       </c>
       <c r="K767" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="L767" t="s">
         <v>834</v>
@@ -60787,7 +60787,7 @@
         <v>823</v>
       </c>
       <c r="K768" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="L768" t="s">
         <v>834</v>
@@ -60829,7 +60829,7 @@
         <v>823</v>
       </c>
       <c r="K769" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="L769" t="s">
         <v>834</v>
@@ -60871,7 +60871,7 @@
         <v>823</v>
       </c>
       <c r="K770" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="L770" t="s">
         <v>834</v>
@@ -62556,7 +62556,7 @@
         <v>596</v>
       </c>
       <c r="D810" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="E810">
         <v>40</v>
@@ -62726,7 +62726,7 @@
         <v>769</v>
       </c>
       <c r="D814" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="E814">
         <v>40</v>
@@ -64915,7 +64915,7 @@
         <v>835</v>
       </c>
       <c r="M865" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="N865">
         <v>50</v>
@@ -64957,7 +64957,7 @@
         <v>835</v>
       </c>
       <c r="M866" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="N866">
         <v>40</v>
@@ -64972,7 +64972,7 @@
         <v>767</v>
       </c>
       <c r="D867" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="E867">
         <v>40</v>
@@ -64999,7 +64999,7 @@
         <v>835</v>
       </c>
       <c r="M867" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="N867">
         <v>40</v>
@@ -65041,7 +65041,7 @@
         <v>835</v>
       </c>
       <c r="M868" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="N868">
         <v>250</v>
@@ -65083,7 +65083,7 @@
         <v>835</v>
       </c>
       <c r="M869" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="N869">
         <v>66.49</v>
@@ -70513,7 +70513,7 @@
         <v>798</v>
       </c>
       <c r="D999" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="E999">
         <v>40</v>
@@ -70683,7 +70683,7 @@
         <v>798</v>
       </c>
       <c r="D1003" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="E1003">
         <v>40</v>
@@ -76198,7 +76198,7 @@
         <v>823</v>
       </c>
       <c r="K1132" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="L1132" t="s">
         <v>834</v>
@@ -76240,7 +76240,7 @@
         <v>823</v>
       </c>
       <c r="K1133" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="L1133" t="s">
         <v>834</v>
@@ -76282,7 +76282,7 @@
         <v>823</v>
       </c>
       <c r="K1134" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="L1134" t="s">
         <v>834</v>
@@ -76324,7 +76324,7 @@
         <v>823</v>
       </c>
       <c r="K1135" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="L1135" t="s">
         <v>834</v>

</xml_diff>